<commit_message>
add excel and pandas
</commit_message>
<xml_diff>
--- a/itr_list.xlsx
+++ b/itr_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\MakeND\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F1421C-C3A9-4B6E-8B2C-F9937717E995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6CB1A7B-2C4C-4872-8465-73D8A76532F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5385" yWindow="2205" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
   <si>
     <t>Фамилия</t>
   </si>
@@ -175,9 +175,6 @@
   </si>
   <si>
     <t>Тищенко</t>
-  </si>
-  <si>
-    <t>Пропустить</t>
   </si>
 </sst>
 </file>
@@ -202,15 +199,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -218,11 +221,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -230,11 +248,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -510,9 +546,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -523,324 +561,348 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="1">
-        <v>1</v>
-      </c>
+      <c r="D2" s="5">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
+      <c r="D3" s="5">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5">
+        <v>1</v>
+      </c>
+      <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
+      <c r="D4" s="5">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="1">
-        <v>1</v>
-      </c>
+      <c r="D5" s="5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="1">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1</v>
-      </c>
+      <c r="D6" s="5">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5">
+        <v>1</v>
+      </c>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="1">
-        <v>1</v>
-      </c>
+      <c r="D7" s="5">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="1">
-        <v>1</v>
-      </c>
+      <c r="D8" s="5">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="1">
-        <v>1</v>
-      </c>
+      <c r="D9" s="5">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="1">
-        <v>1</v>
-      </c>
+      <c r="D10" s="5">
+        <v>1</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="1">
-        <v>1</v>
-      </c>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="1">
-        <v>1</v>
-      </c>
+      <c r="D12" s="5">
+        <v>1</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="1">
-        <v>1</v>
-      </c>
-      <c r="F13" s="1">
+      <c r="D13" s="5"/>
+      <c r="E13" s="5">
+        <v>1</v>
+      </c>
+      <c r="F13" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="1">
-        <v>1</v>
-      </c>
+      <c r="D14" s="5">
+        <v>1</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="1">
-        <v>1</v>
-      </c>
-      <c r="F15" s="1">
+      <c r="D15" s="5"/>
+      <c r="E15" s="5">
+        <v>1</v>
+      </c>
+      <c r="F15" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="1">
-        <v>1</v>
-      </c>
+      <c r="D16" s="5">
+        <v>1</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="1">
-        <v>1</v>
-      </c>
+      <c r="D17" s="5">
+        <v>1</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="1">
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="1">
-        <v>1</v>
-      </c>
-      <c r="E19" s="1">
-        <v>1</v>
-      </c>
+      <c r="D19" s="5">
+        <v>1</v>
+      </c>
+      <c r="E19" s="5">
+        <v>1</v>
+      </c>
+      <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" s="1">
-        <v>1</v>
-      </c>
-      <c r="E21" s="1">
-        <v>1</v>
-      </c>
-      <c r="F21" s="1">
-        <v>1</v>
-      </c>
+      <c r="D20" s="5">
+        <v>1</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F20">
     <sortCondition ref="A1:A20"/>
   </sortState>
+  <conditionalFormatting sqref="D2:F20">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>